<commit_message>
Improve add-storage_v3 for relations and cleanup
</commit_message>
<xml_diff>
--- a/scenario work/China/data/input_data_16_CHN.xlsx
+++ b/scenario work/China/data/input_data_16_CHN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\China\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F383E312-76F5-473A-9447-EA4166635159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F113FDC-74BC-4B69-8FA0-BD549910B80D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="555" windowWidth="20235" windowHeight="11400" activeTab="1" xr2:uid="{821295F0-1D2B-4139-A10C-48DD9AE81549}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20235" windowHeight="11400" activeTab="1" xr2:uid="{821295F0-1D2B-4139-A10C-48DD9AE81549}"/>
   </bookViews>
   <sheets>
     <sheet name="time_steps" sheetId="3" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="85">
   <si>
     <t>Yes</t>
   </si>
@@ -401,6 +401,12 @@
   </si>
   <si>
     <t>time_parent</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>spring-day</t>
   </si>
 </sst>
 </file>
@@ -2978,7 +2984,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="A30" sqref="A30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,7 +3257,7 @@
         <v>76</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3262,7 +3268,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D19">
         <v>0.25</v>
@@ -3276,7 +3282,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20">
         <v>0.25</v>
@@ -3284,17 +3290,16 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D28" si="1">1/16</f>
-        <v>6.25E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3305,10 +3310,10 @@
         <v>76</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D22:D29" si="1">1/16</f>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -3320,7 +3325,7 @@
         <v>76</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
@@ -3335,7 +3340,7 @@
         <v>76</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
@@ -3350,7 +3355,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
@@ -3359,13 +3364,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
@@ -3374,13 +3379,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
@@ -3389,13 +3394,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
@@ -3404,16 +3409,16 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:D36" si="2">1/16</f>
+        <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -3425,10 +3430,10 @@
         <v>75</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D30:D37" si="2">1/16</f>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -3440,7 +3445,7 @@
         <v>75</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
@@ -3455,7 +3460,7 @@
         <v>75</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
@@ -3464,13 +3469,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
@@ -3485,7 +3490,7 @@
         <v>77</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
@@ -3500,7 +3505,7 @@
         <v>77</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
@@ -3515,7 +3520,7 @@
         <v>77</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
@@ -3523,7 +3528,19 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>

</xml_diff>